<commit_message>
9/4 EOD (better late than never)
</commit_message>
<xml_diff>
--- a/Outputs/MassStrataAnalysis.xlsx
+++ b/Outputs/MassStrataAnalysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://acpafl-my.sharepoint.com/personal/agimbel_acpafl_org/Documents/Documents/Aristides/Outputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="11_80A52B3E97213600629E7DC5901DBA82F67CFB9A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E3D8909F-384F-4E31-9B5D-5A687C7BC769}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="11_80A52B3E97213600629E7DC5901DBA82F67CFB9A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ADA2B89E-E1A2-4428-A4D4-81572D8B8670}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AVSA" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,23 @@
     <sheet name="TASA" sheetId="5" r:id="rId5"/>
     <sheet name="MCSA" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -66,24 +82,24 @@
     <t>(0.0, 210000.0]</t>
   </si>
   <si>
+    <t>{'PRB': -0.09202983846653265, 'Sig': 1.9099948957354152e-237}</t>
+  </si>
+  <si>
     <t>(210000.0, 295835.0]</t>
   </si>
   <si>
+    <t>{'PRB': -0.5146775996459074, 'Sig': 0.0}</t>
+  </si>
+  <si>
     <t>(295835.0, 423131.0]</t>
   </si>
   <si>
+    <t>{'PRB': -0.5491915938654108, 'Sig': 0.0}</t>
+  </si>
+  <si>
     <t>(423131.0, inf]</t>
   </si>
   <si>
-    <t>{'PRB': -0.09202983846653265, 'Sig': 1.9099948957354152e-237}</t>
-  </si>
-  <si>
-    <t>{'PRB': -0.5146775996459074, 'Sig': 0.0}</t>
-  </si>
-  <si>
-    <t>{'PRB': -0.5491915938654108, 'Sig': 0.0}</t>
-  </si>
-  <si>
     <t>{'PRB': -0.28301298974212663, 'Sig': 1.8869860981146176e-132}</t>
   </si>
   <si>
@@ -93,42 +109,42 @@
     <t>(0.0, 1000.0]</t>
   </si>
   <si>
+    <t>{'PRB': -0.0069563928537033914, 'Sig': 0.6230698469232488}</t>
+  </si>
+  <si>
     <t>(1000.0, 1500.0]</t>
   </si>
   <si>
+    <t>{'PRB': -0.07099279286801072, 'Sig': 3.9470593519799304e-50}</t>
+  </si>
+  <si>
     <t>(1500.0, 2000.0]</t>
   </si>
   <si>
+    <t>{'PRB': -0.13593372608233778, 'Sig': 4.177883163955743e-245}</t>
+  </si>
+  <si>
     <t>(2000.0, 2500.0]</t>
   </si>
   <si>
+    <t>{'PRB': -0.142027187815009, 'Sig': 5.843080481830932e-132}</t>
+  </si>
+  <si>
     <t>(2500.0, 3000.0]</t>
   </si>
   <si>
+    <t>{'PRB': -0.12381922776084937, 'Sig': 7.145245007282648e-53}</t>
+  </si>
+  <si>
     <t>(3000.0, 3500.0]</t>
   </si>
   <si>
+    <t>{'PRB': -0.08117063815094207, 'Sig': 1.436819064556789e-17}</t>
+  </si>
+  <si>
     <t>(3500.0, inf]</t>
   </si>
   <si>
-    <t>{'PRB': -0.0069563928537033914, 'Sig': 0.6230698469232488}</t>
-  </si>
-  <si>
-    <t>{'PRB': -0.07099279286801072, 'Sig': 3.9470593519799304e-50}</t>
-  </si>
-  <si>
-    <t>{'PRB': -0.13593372608233778, 'Sig': 4.177883163955743e-245}</t>
-  </si>
-  <si>
-    <t>{'PRB': -0.142027187815009, 'Sig': 5.843080481830932e-132}</t>
-  </si>
-  <si>
-    <t>{'PRB': -0.12381922776084937, 'Sig': 7.145245007282648e-53}</t>
-  </si>
-  <si>
-    <t>{'PRB': -0.08117063815094207, 'Sig': 1.436819064556789e-17}</t>
-  </si>
-  <si>
     <t>{'PRB': -0.028741279821081805, 'Sig': 7.419212596183356e-05}</t>
   </si>
   <si>
@@ -138,30 +154,30 @@
     <t>(0.0, 0.19]</t>
   </si>
   <si>
+    <t>{'PRB': 0.009019544347908783, 'Sig': 0.00016275844834976578}</t>
+  </si>
+  <si>
     <t>(0.19, 0.2]</t>
   </si>
   <si>
+    <t>{'PRB': -0.07708298382846221, 'Sig': 6.445801420824754e-39}</t>
+  </si>
+  <si>
     <t>(0.2, 0.34]</t>
   </si>
   <si>
+    <t>{'PRB': -0.05100424058285153, 'Sig': 8.942776132830577e-125}</t>
+  </si>
+  <si>
     <t>(0.34, 0.35]</t>
   </si>
   <si>
+    <t>{'PRB': -0.033888115253019664, 'Sig': 0.00041876008001703766}</t>
+  </si>
+  <si>
     <t>(0.35, inf]</t>
   </si>
   <si>
-    <t>{'PRB': 0.009019544347908783, 'Sig': 0.00016275844834976578}</t>
-  </si>
-  <si>
-    <t>{'PRB': -0.07708298382846221, 'Sig': 6.445801420824754e-39}</t>
-  </si>
-  <si>
-    <t>{'PRB': -0.05100424058285153, 'Sig': 8.942776132830577e-125}</t>
-  </si>
-  <si>
-    <t>{'PRB': -0.033888115253019664, 'Sig': 0.00041876008001703766}</t>
-  </si>
-  <si>
     <t>{'PRB': -0.00311516216481913, 'Sig': 0.17887950254408694}</t>
   </si>
   <si>
@@ -192,66 +208,66 @@
     <t>ALACHUA</t>
   </si>
   <si>
+    <t>{'PRB': 0.04203112160851699, 'Sig': 5.327537839858841e-16}</t>
+  </si>
+  <si>
     <t>ARCHER</t>
   </si>
   <si>
+    <t>{'PRB': 0.023922831134888946, 'Sig': 0.31264300287815283}</t>
+  </si>
+  <si>
     <t>GAINESVILLE</t>
   </si>
   <si>
+    <t>{'PRB': -0.05741227608996373, 'Sig': 2.9226250078816448e-170}</t>
+  </si>
+  <si>
     <t>HAWTHORNE</t>
   </si>
   <si>
+    <t>{'PRB': -0.024448442961555364, 'Sig': 0.05949798254603737}</t>
+  </si>
+  <si>
     <t>HIGH SPRINGS</t>
   </si>
   <si>
+    <t>{'PRB': -0.09376882055715562, 'Sig': 1.1166561507377886e-22}</t>
+  </si>
+  <si>
     <t>LACROSSE</t>
   </si>
   <si>
+    <t>{'PRB': 0.018432232628190447, 'Sig': 0.6876601760903462}</t>
+  </si>
+  <si>
     <t>MICANOPY</t>
   </si>
   <si>
+    <t>{'PRB': 0.0401470219551682, 'Sig': 0.060867785803662776}</t>
+  </si>
+  <si>
     <t>NEWBERRY</t>
   </si>
   <si>
+    <t>{'PRB': -0.06452837481935612, 'Sig': 2.398172430653273e-14}</t>
+  </si>
+  <si>
     <t>ST. JOHN'S</t>
   </si>
   <si>
+    <t>{'PRB': 0.030133975338668458, 'Sig': 7.439376019286784e-62}</t>
+  </si>
+  <si>
     <t>SUWANNEE</t>
   </si>
   <si>
+    <t>{'PRB': -0.03358079633541246, 'Sig': 6.353524226787923e-15}</t>
+  </si>
+  <si>
     <t>WALDO</t>
   </si>
   <si>
-    <t>{'PRB': 0.04203112160851699, 'Sig': 5.327537839858841e-16}</t>
-  </si>
-  <si>
-    <t>{'PRB': 0.023922831134888946, 'Sig': 0.31264300287815283}</t>
-  </si>
-  <si>
-    <t>{'PRB': -0.05741227608996373, 'Sig': 2.9226250078816448e-170}</t>
-  </si>
-  <si>
-    <t>{'PRB': -0.024448442961555364, 'Sig': 0.05949798254603737}</t>
-  </si>
-  <si>
-    <t>{'PRB': -0.09376882055715562, 'Sig': 1.1166561507377886e-22}</t>
-  </si>
-  <si>
-    <t>{'PRB': 0.018432232628190447, 'Sig': 0.6876601760903462}</t>
-  </si>
-  <si>
-    <t>{'PRB': 0.0401470219551682, 'Sig': 0.060867785803662776}</t>
-  </si>
-  <si>
-    <t>{'PRB': -0.06452837481935612, 'Sig': 2.398172430653273e-14}</t>
-  </si>
-  <si>
-    <t>{'PRB': 0.030133975338668458, 'Sig': 7.439376019286784e-62}</t>
-  </si>
-  <si>
-    <t>{'PRB': -0.03358079633541246, 'Sig': 6.353524226787923e-15}</t>
-  </si>
-  <si>
     <t>{'PRB': 0.12238633315537786, 'Sig': 0.00013763876266952856}</t>
   </si>
   <si>
@@ -261,136 +277,136 @@
     <t>HighSprings_A</t>
   </si>
   <si>
+    <t>{'PRB': -0.032422850288205164, 'Sig': 1.0319667923159685e-22}</t>
+  </si>
+  <si>
     <t>HighSprings_B</t>
   </si>
   <si>
+    <t>{'PRB': -0.023109496074456552, 'Sig': 2.4144547790969165e-33}</t>
+  </si>
+  <si>
     <t>HighSprings_C</t>
   </si>
   <si>
+    <t>{'PRB': -0.058856600689720685, 'Sig': 0.09797558511477819}</t>
+  </si>
+  <si>
     <t>HighSprings_D</t>
   </si>
   <si>
+    <t>{'PRB': -0.017422764376869737, 'Sig': 0.5724740224410586}</t>
+  </si>
+  <si>
     <t>HighSprings_E</t>
   </si>
   <si>
+    <t>{'PRB': -0.008421481032782206, 'Sig': 0.8298216687537444}</t>
+  </si>
+  <si>
     <t>HighSprings_F</t>
   </si>
   <si>
+    <t>{'PRB': 0.12448392197906735, 'Sig': 3.679004576306938e-26}</t>
+  </si>
+  <si>
     <t>MidtownEast_A</t>
   </si>
   <si>
+    <t>{'PRB': 0.0797870294570036, 'Sig': 7.265507978396119e-16}</t>
+  </si>
+  <si>
     <t>MidtownEast_B</t>
   </si>
   <si>
+    <t>{'PRB': -0.0635004699350393, 'Sig': 1.047697082224165e-28}</t>
+  </si>
+  <si>
     <t>MidtownEast_C</t>
   </si>
   <si>
+    <t>{'PRB': 0.001441768380499876, 'Sig': 0.8384929786610348}</t>
+  </si>
+  <si>
     <t>MidtownEast_D</t>
   </si>
   <si>
+    <t>{'PRB': 0.037938214678295994, 'Sig': 0.00028847663233826196}</t>
+  </si>
+  <si>
     <t>MidtownEast_E</t>
   </si>
   <si>
+    <t>{'PRB': 0.04408555709450266, 'Sig': 0.0005924034720723206}</t>
+  </si>
+  <si>
     <t>MidtownEast_F</t>
   </si>
   <si>
+    <t>{'PRB': -0.0053580283508415875, 'Sig': 0.8728640247478588}</t>
+  </si>
+  <si>
     <t>Springtree_A</t>
   </si>
   <si>
+    <t>{'PRB': 0.12102381854999328, 'Sig': 4.029597946170329e-17}</t>
+  </si>
+  <si>
     <t>Springtree_B</t>
   </si>
   <si>
+    <t>{'PRB': -0.059141549854705086, 'Sig': 7.583747514115197e-62}</t>
+  </si>
+  <si>
     <t>Springtree_C</t>
   </si>
   <si>
+    <t>{'PRB': 0.1068974268331364, 'Sig': 3.183116730056111e-15}</t>
+  </si>
+  <si>
     <t>Tioga_A</t>
   </si>
   <si>
+    <t>{'PRB': 0.01795723351760968, 'Sig': 0.03994597491874655}</t>
+  </si>
+  <si>
     <t>Tioga_B</t>
   </si>
   <si>
+    <t>{'PRB': 0.05018591207415716, 'Sig': 7.454969007033319e-05}</t>
+  </si>
+  <si>
     <t>WaldoRural_A</t>
   </si>
   <si>
+    <t>{'PRB': 0.03743631587026259, 'Sig': 0.16700689062152826}</t>
+  </si>
+  <si>
     <t>WaldoRural_B</t>
   </si>
   <si>
+    <t>{'PRB': 0.06491100467590559, 'Sig': 0.0034810018333884035}</t>
+  </si>
+  <si>
     <t>WaldoRural_C</t>
   </si>
   <si>
+    <t>{'PRB': 0.07453675871288687, 'Sig': 2.30803019799313e-09}</t>
+  </si>
+  <si>
     <t>swNewberry_A</t>
   </si>
   <si>
+    <t>{'PRB': -0.07181049863542563, 'Sig': 1.125008990428273e-14}</t>
+  </si>
+  <si>
     <t>swNewberry_B</t>
   </si>
   <si>
+    <t>{'PRB': -0.0062271572205909445, 'Sig': 0.6373248677963328}</t>
+  </si>
+  <si>
     <t>swNewberry_C</t>
-  </si>
-  <si>
-    <t>{'PRB': -0.032422850288205164, 'Sig': 1.0319667923159685e-22}</t>
-  </si>
-  <si>
-    <t>{'PRB': -0.023109496074456552, 'Sig': 2.4144547790969165e-33}</t>
-  </si>
-  <si>
-    <t>{'PRB': -0.058856600689720685, 'Sig': 0.09797558511477819}</t>
-  </si>
-  <si>
-    <t>{'PRB': -0.017422764376869737, 'Sig': 0.5724740224410586}</t>
-  </si>
-  <si>
-    <t>{'PRB': -0.008421481032782206, 'Sig': 0.8298216687537444}</t>
-  </si>
-  <si>
-    <t>{'PRB': 0.12448392197906735, 'Sig': 3.679004576306938e-26}</t>
-  </si>
-  <si>
-    <t>{'PRB': 0.0797870294570036, 'Sig': 7.265507978396119e-16}</t>
-  </si>
-  <si>
-    <t>{'PRB': -0.0635004699350393, 'Sig': 1.047697082224165e-28}</t>
-  </si>
-  <si>
-    <t>{'PRB': 0.001441768380499876, 'Sig': 0.8384929786610348}</t>
-  </si>
-  <si>
-    <t>{'PRB': 0.037938214678295994, 'Sig': 0.00028847663233826196}</t>
-  </si>
-  <si>
-    <t>{'PRB': 0.04408555709450266, 'Sig': 0.0005924034720723206}</t>
-  </si>
-  <si>
-    <t>{'PRB': -0.0053580283508415875, 'Sig': 0.8728640247478588}</t>
-  </si>
-  <si>
-    <t>{'PRB': 0.12102381854999328, 'Sig': 4.029597946170329e-17}</t>
-  </si>
-  <si>
-    <t>{'PRB': -0.059141549854705086, 'Sig': 7.583747514115197e-62}</t>
-  </si>
-  <si>
-    <t>{'PRB': 0.1068974268331364, 'Sig': 3.183116730056111e-15}</t>
-  </si>
-  <si>
-    <t>{'PRB': 0.01795723351760968, 'Sig': 0.03994597491874655}</t>
-  </si>
-  <si>
-    <t>{'PRB': 0.05018591207415716, 'Sig': 7.454969007033319e-05}</t>
-  </si>
-  <si>
-    <t>{'PRB': 0.03743631587026259, 'Sig': 0.16700689062152826}</t>
-  </si>
-  <si>
-    <t>{'PRB': 0.06491100467590559, 'Sig': 0.0034810018333884035}</t>
-  </si>
-  <si>
-    <t>{'PRB': 0.07453675871288687, 'Sig': 2.30803019799313e-09}</t>
-  </si>
-  <si>
-    <t>{'PRB': -0.07181049863542563, 'Sig': 1.125008990428273e-14}</t>
-  </si>
-  <si>
-    <t>{'PRB': -0.0062271572205909445, 'Sig': 0.6373248677963328}</t>
   </si>
   <si>
     <t>{'PRB': 0.10427856703831585, 'Sig': 1.1199994926613015e-20}</t>
@@ -400,7 +416,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -763,9 +779,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
@@ -779,7 +797,7 @@
     <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -817,7 +835,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -840,7 +858,7 @@
         <v>14.54479896868625</v>
       </c>
       <c r="H2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I2">
         <v>0.84826297780520954</v>
@@ -855,9 +873,9 @@
         <v>1.1506264868950959</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B3">
         <v>15726</v>
@@ -878,7 +896,7 @@
         <v>10.80991142802791</v>
       </c>
       <c r="H3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I3">
         <v>0.87157031213531921</v>
@@ -893,9 +911,9 @@
         <v>1.1405355792027201</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B4">
         <v>8477</v>
@@ -916,7 +934,7 @@
         <v>11.48225348243119</v>
       </c>
       <c r="H4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I4">
         <v>0.8849682729287478</v>
@@ -931,9 +949,9 @@
         <v>1.1356288547414799</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B5">
         <v>3905</v>
@@ -978,11 +996,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:J1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="30.5703125" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="8" max="8" width="58.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" customWidth="1"/>
+    <col min="10" max="10" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.85546875" customWidth="1"/>
+    <col min="12" max="12" width="17.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -1020,7 +1049,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -1043,7 +1072,7 @@
         <v>23.706873752088018</v>
       </c>
       <c r="H2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="I2">
         <v>0.85351303305221382</v>
@@ -1058,9 +1087,9 @@
         <v>1.1813765002361269</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B3">
         <v>19141</v>
@@ -1081,7 +1110,7 @@
         <v>13.166959080940011</v>
       </c>
       <c r="H3" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="I3">
         <v>0.88865314948714635</v>
@@ -1096,9 +1125,9 @@
         <v>1.1174428916385959</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B4">
         <v>16036</v>
@@ -1119,7 +1148,7 @@
         <v>10.877873796381349</v>
       </c>
       <c r="H4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="I4">
         <v>0.87086299179855231</v>
@@ -1134,9 +1163,9 @@
         <v>1.144242932773391</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B5">
         <v>9151</v>
@@ -1157,7 +1186,7 @@
         <v>11.611259247572301</v>
       </c>
       <c r="H5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I5">
         <v>0.86167168554874818</v>
@@ -1172,9 +1201,9 @@
         <v>1.16637113543161</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B6">
         <v>4517</v>
@@ -1195,7 +1224,7 @@
         <v>11.62950431168125</v>
       </c>
       <c r="H6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I6">
         <v>0.86867984158928058</v>
@@ -1210,9 +1239,9 @@
         <v>1.1627909659180129</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B7">
         <v>2104</v>
@@ -1233,7 +1262,7 @@
         <v>11.061648543283249</v>
       </c>
       <c r="H7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I7">
         <v>0.87093559343621552</v>
@@ -1248,9 +1277,9 @@
         <v>1.150802982568603</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="B8">
         <v>2068</v>
@@ -1297,9 +1326,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>35</v>
       </c>
@@ -1337,7 +1366,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -1360,7 +1389,7 @@
         <v>12.62251583353499</v>
       </c>
       <c r="H2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="I2">
         <v>0.87242147125200764</v>
@@ -1375,9 +1404,9 @@
         <v>1.1452487176098729</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B3">
         <v>1740</v>
@@ -1398,7 +1427,7 @@
         <v>9.826540131090006</v>
       </c>
       <c r="H3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="I3">
         <v>0.89740307592060586</v>
@@ -1413,9 +1442,9 @@
         <v>1.0990310784415791</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B4">
         <v>17725</v>
@@ -1436,7 +1465,7 @@
         <v>10.749116487573261</v>
       </c>
       <c r="H4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I4">
         <v>0.90215081751563975</v>
@@ -1451,9 +1480,9 @@
         <v>1.1051960771121301</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B5">
         <v>792</v>
@@ -1474,7 +1503,7 @@
         <v>9.6472961257984693</v>
       </c>
       <c r="H5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I5">
         <v>0.88131427633262782</v>
@@ -1489,9 +1518,9 @@
         <v>1.1310678813234669</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B6">
         <v>22201</v>
@@ -1538,9 +1567,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>46</v>
       </c>
@@ -1578,7 +1607,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12">
       <c r="A2">
         <v>0.75</v>
       </c>
@@ -1616,7 +1645,7 @@
         <v>1.2750649781020249</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12">
       <c r="A3">
         <v>0.9</v>
       </c>
@@ -1654,7 +1683,7 @@
         <v>1.3335077006085889</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1692,7 +1721,7 @@
         <v>1.1293903867602779</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12">
       <c r="A5">
         <v>1.1499999999999999</v>
       </c>
@@ -1730,7 +1759,7 @@
         <v>1.177571694456409</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12">
       <c r="A6">
         <v>1.4</v>
       </c>
@@ -1768,7 +1797,7 @@
         <v>1.168172282645237</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12">
       <c r="A7">
         <v>1.7</v>
       </c>
@@ -1817,9 +1846,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>53</v>
       </c>
@@ -1857,7 +1886,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>54</v>
       </c>
@@ -1880,7 +1909,7 @@
         <v>11.54053988118577</v>
       </c>
       <c r="H2" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="I2">
         <v>0.86071685298859268</v>
@@ -1895,9 +1924,9 @@
         <v>1.16495313622122</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B3">
         <v>311</v>
@@ -1918,7 +1947,7 @@
         <v>16.752935980870859</v>
       </c>
       <c r="H3" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="I3">
         <v>0.73451322560060783</v>
@@ -1933,9 +1962,9 @@
         <v>1.3591996801003079</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B4">
         <v>23300</v>
@@ -1956,7 +1985,7 @@
         <v>12.51844373338402</v>
       </c>
       <c r="H4" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="I4">
         <v>0.87980431354334099</v>
@@ -1971,9 +2000,9 @@
         <v>1.128895376564433</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B5">
         <v>541</v>
@@ -1994,7 +2023,7 @@
         <v>12.11530543829574</v>
       </c>
       <c r="H5" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="I5">
         <v>0.97086552961941985</v>
@@ -2009,9 +2038,9 @@
         <v>1.0392753891033899</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B6">
         <v>2023</v>
@@ -2032,7 +2061,7 @@
         <v>11.459896774147269</v>
       </c>
       <c r="H6" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="I6">
         <v>0.87528990256003159</v>
@@ -2047,9 +2076,9 @@
         <v>1.1636581693555861</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12">
       <c r="A7" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="B7">
         <v>48</v>
@@ -2070,7 +2099,7 @@
         <v>11.880610196854141</v>
       </c>
       <c r="H7" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="I7">
         <v>0.67164929191979461</v>
@@ -2085,9 +2114,9 @@
         <v>1.550622076823863</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="B8">
         <v>250</v>
@@ -2108,7 +2137,7 @@
         <v>13.51386725980114</v>
       </c>
       <c r="H8" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="I8">
         <v>0.8661657860655575</v>
@@ -2123,9 +2152,9 @@
         <v>1.17993484561864</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12">
       <c r="A9" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="B9">
         <v>1859</v>
@@ -2146,7 +2175,7 @@
         <v>9.5182763490848501</v>
       </c>
       <c r="H9" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="I9">
         <v>0.86240375116012302</v>
@@ -2161,9 +2190,9 @@
         <v>1.1390492861773029</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12">
       <c r="A10" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="B10">
         <v>17955</v>
@@ -2184,7 +2213,7 @@
         <v>12.23720713973298</v>
       </c>
       <c r="H10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I10">
         <v>0.88135038141933941</v>
@@ -2199,9 +2228,9 @@
         <v>1.137378927137235</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12">
       <c r="A11" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="B11">
         <v>8203</v>
@@ -2222,7 +2251,7 @@
         <v>16.072847969223002</v>
       </c>
       <c r="H11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I11">
         <v>0.84890505724742049</v>
@@ -2237,9 +2266,9 @@
         <v>1.1931050575472939</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12">
       <c r="A12" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="B12">
         <v>200</v>
@@ -2286,9 +2315,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>76</v>
       </c>
@@ -2326,7 +2355,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>77</v>
       </c>
@@ -2349,7 +2378,7 @@
         <v>9.9678077784739489</v>
       </c>
       <c r="H2" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="I2">
         <v>0.88757875648922702</v>
@@ -2364,9 +2393,9 @@
         <v>1.123350613304376</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B3">
         <v>22019</v>
@@ -2387,7 +2416,7 @@
         <v>11.36394566655529</v>
       </c>
       <c r="H3" t="s">
-        <v>101</v>
+        <v>80</v>
       </c>
       <c r="I3">
         <v>0.86556207193318879</v>
@@ -2402,9 +2431,9 @@
         <v>1.1573643602927981</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B4">
         <v>168</v>
@@ -2425,7 +2454,7 @@
         <v>16.39361934073202</v>
       </c>
       <c r="H4" t="s">
-        <v>102</v>
+        <v>82</v>
       </c>
       <c r="I4">
         <v>0.79763759796363642</v>
@@ -2440,9 +2469,9 @@
         <v>1.3163506675528629</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B5">
         <v>217</v>
@@ -2463,7 +2492,7 @@
         <v>11.539726488756861</v>
       </c>
       <c r="H5" t="s">
-        <v>103</v>
+        <v>84</v>
       </c>
       <c r="I5">
         <v>0.98192304656411</v>
@@ -2478,9 +2507,9 @@
         <v>1.0274025283425201</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="B6">
         <v>487</v>
@@ -2501,7 +2530,7 @@
         <v>35.775091861445581</v>
       </c>
       <c r="H6" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
       <c r="I6">
         <v>1.0132518954387579</v>
@@ -2516,9 +2545,9 @@
         <v>1.154618813669311</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12">
       <c r="A7" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="B7">
         <v>1300</v>
@@ -2539,7 +2568,7 @@
         <v>14.718291746009349</v>
       </c>
       <c r="H7" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="I7">
         <v>0.91524810876778728</v>
@@ -2554,9 +2583,9 @@
         <v>1.0670234926851121</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="B8">
         <v>2946</v>
@@ -2577,7 +2606,7 @@
         <v>20.92717633761804</v>
       </c>
       <c r="H8" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="I8">
         <v>0.86958919582277572</v>
@@ -2592,9 +2621,9 @@
         <v>1.1767570517191299</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12">
       <c r="A9" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="B9">
         <v>2009</v>
@@ -2615,7 +2644,7 @@
         <v>10.29289283479082</v>
       </c>
       <c r="H9" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="I9">
         <v>0.87932530406735376</v>
@@ -2630,9 +2659,9 @@
         <v>1.1201282965930011</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12">
       <c r="A10" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="B10">
         <v>6642</v>
@@ -2653,7 +2682,7 @@
         <v>16.86145818577139</v>
       </c>
       <c r="H10" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="I10">
         <v>0.90816107514015643</v>
@@ -2668,9 +2697,9 @@
         <v>1.1006504604315319</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12">
       <c r="A11" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="B11">
         <v>935</v>
@@ -2691,7 +2720,7 @@
         <v>15.34836542714471</v>
       </c>
       <c r="H11" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="I11">
         <v>0.83733121717426129</v>
@@ -2706,9 +2735,9 @@
         <v>1.2234044586996231</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12">
       <c r="A12" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="B12">
         <v>318</v>
@@ -2729,7 +2758,7 @@
         <v>7.0902704959717067</v>
       </c>
       <c r="H12" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="I12">
         <v>0.87520040374148178</v>
@@ -2744,9 +2773,9 @@
         <v>1.145865982627887</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12">
       <c r="A13" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="B13">
         <v>80</v>
@@ -2767,7 +2796,7 @@
         <v>6.8459193960402196</v>
       </c>
       <c r="H13" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="I13">
         <v>0.8810459763539793</v>
@@ -2782,9 +2811,9 @@
         <v>1.1360599781298031</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12">
       <c r="A14" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="B14">
         <v>715</v>
@@ -2805,7 +2834,7 @@
         <v>8.0923200594776681</v>
       </c>
       <c r="H14" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="I14">
         <v>0.84812551552430993</v>
@@ -2820,9 +2849,9 @@
         <v>1.1552809362493259</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12">
       <c r="A15" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="B15">
         <v>6243</v>
@@ -2843,7 +2872,7 @@
         <v>7.9795867351152356</v>
       </c>
       <c r="H15" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="I15">
         <v>0.87885316562335691</v>
@@ -2858,9 +2887,9 @@
         <v>1.1272163223072771</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12">
       <c r="A16" t="s">
-        <v>91</v>
+        <v>105</v>
       </c>
       <c r="B16">
         <v>418</v>
@@ -2881,7 +2910,7 @@
         <v>13.02006367564006</v>
       </c>
       <c r="H16" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="I16">
         <v>0.82440011900894294</v>
@@ -2896,9 +2925,9 @@
         <v>1.2491410581548199</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12">
       <c r="A17" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
       <c r="B17">
         <v>592</v>
@@ -2919,7 +2948,7 @@
         <v>8.5514775537018082</v>
       </c>
       <c r="H17" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="I17">
         <v>0.91607435273297011</v>
@@ -2934,9 +2963,9 @@
         <v>1.101996255440695</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12">
       <c r="A18" t="s">
-        <v>93</v>
+        <v>109</v>
       </c>
       <c r="B18">
         <v>525</v>
@@ -2957,7 +2986,7 @@
         <v>11.402805489565591</v>
       </c>
       <c r="H18" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="I18">
         <v>0.89224200300616152</v>
@@ -2972,9 +3001,9 @@
         <v>1.1395284038329461</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12">
       <c r="A19" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
       <c r="B19">
         <v>271</v>
@@ -2995,7 +3024,7 @@
         <v>17.06746875815297</v>
       </c>
       <c r="H19" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="I19">
         <v>1.0169521738936389</v>
@@ -3010,9 +3039,9 @@
         <v>0.97543779620312099</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12">
       <c r="A20" t="s">
-        <v>95</v>
+        <v>113</v>
       </c>
       <c r="B20">
         <v>271</v>
@@ -3033,7 +3062,7 @@
         <v>13.032738816135961</v>
       </c>
       <c r="H20" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="I20">
         <v>1.047185458541315</v>
@@ -3048,9 +3077,9 @@
         <v>0.96116417143013755</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12">
       <c r="A21" t="s">
-        <v>96</v>
+        <v>115</v>
       </c>
       <c r="B21">
         <v>1837</v>
@@ -3071,7 +3100,7 @@
         <v>23.261176603402781</v>
       </c>
       <c r="H21" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="I21">
         <v>0.84699690444404008</v>
@@ -3086,9 +3115,9 @@
         <v>1.2691585093836171</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12">
       <c r="A22" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
       <c r="B22">
         <v>1847</v>
@@ -3109,7 +3138,7 @@
         <v>9.6722804760860903</v>
       </c>
       <c r="H22" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I22">
         <v>0.86515471523086795</v>
@@ -3124,9 +3153,9 @@
         <v>1.137797002363401</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12">
       <c r="A23" t="s">
-        <v>98</v>
+        <v>119</v>
       </c>
       <c r="B23">
         <v>1790</v>
@@ -3147,7 +3176,7 @@
         <v>11.046698665554731</v>
       </c>
       <c r="H23" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I23">
         <v>0.86844385367377519</v>
@@ -3162,9 +3191,9 @@
         <v>1.1544453376561421</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12">
       <c r="A24" t="s">
-        <v>99</v>
+        <v>121</v>
       </c>
       <c r="B24">
         <v>839</v>

</xml_diff>